<commit_message>
two-month forecast, shiny, tweaked regression
</commit_message>
<xml_diff>
--- a/Monthly GDP for Project.xlsx
+++ b/Monthly GDP for Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesch\OneDrive\Documents\RStudio\recession_predictR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369EA232-5A90-4FED-9507-334AB3BF0F1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394476E0-527A-4C6F-8F23-D4027347555C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly GDP" sheetId="4" r:id="rId1"/>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{193AEE4A-BA1F-DD4C-80AC-7DE24BE31259}">
   <dimension ref="A1:E877"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A858" workbookViewId="0">
-      <selection activeCell="A878" sqref="A878"/>
+    <sheetView tabSelected="1" topLeftCell="A848" workbookViewId="0">
+      <selection activeCell="F874" sqref="F874"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14413,7 +14413,7 @@
         <v>17764.792999999998</v>
       </c>
       <c r="C836">
-        <f t="shared" ref="C836:C874" si="26">(LN(B836)-LN(B835))*12</f>
+        <f t="shared" ref="C836:C877" si="26">(LN(B836)-LN(B835))*12</f>
         <v>2.0091798277015016E-2</v>
       </c>
       <c r="D836">
@@ -14626,7 +14626,7 @@
         <v>3.1424829752459971E-2</v>
       </c>
       <c r="D847">
-        <f t="shared" ref="D847:D874" si="27">(B847-B835)/B835</f>
+        <f t="shared" ref="D847:D877" si="27">(B847-B835)/B835</f>
         <v>2.4160260058683734E-2</v>
       </c>
       <c r="E847">
@@ -15150,6 +15150,17 @@
       <c r="A875" s="5">
         <v>43800</v>
       </c>
+      <c r="B875">
+        <v>19256.189999999999</v>
+      </c>
+      <c r="C875">
+        <f t="shared" si="26"/>
+        <v>2.1344061579902984E-2</v>
+      </c>
+      <c r="D875">
+        <f t="shared" si="27"/>
+        <v>2.2554333150713576E-2</v>
+      </c>
       <c r="E875">
         <v>0.17600000000000002</v>
       </c>
@@ -15158,6 +15169,17 @@
       <c r="A876" s="5">
         <v>43831</v>
       </c>
+      <c r="B876">
+        <v>19252.03</v>
+      </c>
+      <c r="C876">
+        <f t="shared" si="26"/>
+        <v>-2.5926932064948005E-3</v>
+      </c>
+      <c r="D876">
+        <f t="shared" si="27"/>
+        <v>1.973900612149683E-2</v>
+      </c>
       <c r="E876">
         <v>0.17399999999999999</v>
       </c>
@@ -15165,6 +15187,17 @@
     <row r="877" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A877" s="5">
         <v>43862</v>
+      </c>
+      <c r="B877">
+        <v>19370.830000000002</v>
+      </c>
+      <c r="C877">
+        <f t="shared" si="26"/>
+        <v>7.3821798591048093E-2</v>
+      </c>
+      <c r="D877">
+        <f t="shared" si="27"/>
+        <v>2.3434374963842017E-2</v>
       </c>
       <c r="E877">
         <v>0.17</v>

</xml_diff>